<commit_message>
bug fixed for FORMULA cell value
</commit_message>
<xml_diff>
--- a/src/main/java/com/excel/lib/util/SampleExcel.xlsx
+++ b/src/main/java/com/excel/lib/util/SampleExcel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NaveenKhunteta/Documents/workspace/ExcelUtil/src/main/java/com/excel/lib/util/"/>
     </mc:Choice>
@@ -13,9 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="Naveen" r:id="rId5" sheetId="2"/>
-    <sheet name="Naveen1" r:id="rId6" sheetId="3"/>
-    <sheet name="Naveen2" r:id="rId7" sheetId="4"/>
+    <sheet name="Naveen" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
@@ -41,26 +39,16 @@
     <t>test123</t>
   </si>
   <si>
-    <t>tom123</t>
+    <t>wsss</t>
   </si>
   <si>
-    <t>ppp</t>
-  </si>
-  <si>
-    <t>kkk</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>pass</t>
+    <t>99999</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -90,11 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,18 +358,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.015625" collapsed="true"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,20 +377,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <f>SUM(10+40)</f>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -413,37 +400,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>